<commit_message>
export data statistical excel
</commit_message>
<xml_diff>
--- a/BE/src/main/resources/jxls/api_data.xlsx
+++ b/BE/src/main/resources/jxls/api_data.xlsx
@@ -1,35 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5018FA84-2FB2-4EDD-B9AF-B41DD1AC57FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Thống kê" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,11 +40,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="D4")</t>
+jx:area(lastCell="F5")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A3" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -73,7 +64,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="apiData" var="data" lastCell="D4")</t>
+jx:each(items="apiData" var="data" lastCell="F5")
+jx:each(items="apiData2" var="data2" lastCell="F5")</t>
         </r>
       </text>
     </comment>
@@ -82,31 +74,50 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>${data.code}</t>
-  </si>
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>${data.number}</t>
-  </si>
-  <si>
-    <t>${data.errors}</t>
-  </si>
-  <si>
-    <t>Thống kê doanh thu</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+  <si>
+    <t>Tổng Đơn Hàng Tháng Này</t>
+  </si>
+  <si>
+    <t>Tổng Doanh Thu Tháng Này</t>
+  </si>
+  <si>
+    <t>Tổng Đơn Hàng Hôm Nay</t>
+  </si>
+  <si>
+    <t>Tổng Doanh Thu Hôm Nay</t>
+  </si>
+  <si>
+    <t>Tổng Sản Phẩm Bán Ra Tháng Này</t>
+  </si>
+  <si>
+    <t>${data2.totalBill}  Đơn Hàng</t>
+  </si>
+  <si>
+    <t>${data.totalBillToday}  Đơn Hàng</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ${data2.totalProduct}  Sản phẩm</t>
+  </si>
+  <si>
+    <t>THỐNG KÊ DOANH THU, HOÁ ĐƠN, SẢN PHẨM BÁN RA</t>
+  </si>
+  <si>
+    <t>${data2.totalBillAmount}</t>
+  </si>
+  <si>
+    <t>${data.totalBillAmountToday}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,14 +137,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -144,14 +147,35 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFC00000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,18 +184,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.39997558519241921"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -183,52 +231,47 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
+      <right/>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -245,9 +288,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -285,9 +328,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,7 +365,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,7 +400,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -530,53 +573,81 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="2.5546875" customWidth="1"/>
+    <col min="2" max="2" width="38.44140625" customWidth="1"/>
     <col min="3" max="3" width="38.88671875" customWidth="1"/>
-    <col min="4" max="4" width="79.88671875" customWidth="1"/>
+    <col min="4" max="4" width="38.109375" customWidth="1"/>
+    <col min="5" max="5" width="37.21875" customWidth="1"/>
+    <col min="6" max="6" width="47.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3"/>
-      <c r="B1" s="6" t="s">
-        <v>4</v>
-      </c>
+    <row r="1" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:4" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A4" s="5"/>
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix bug  : excel  + update trả hàng
</commit_message>
<xml_diff>
--- a/BE/src/main/resources/jxls/api_data.xlsx
+++ b/BE/src/main/resources/jxls/api_data.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A429D8BB-B328-4A5D-BC03-39C06435834D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Thống kê" sheetId="3" r:id="rId1"/>
@@ -15,12 +14,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -44,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="A4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -66,7 +65,31 @@
           <t xml:space="preserve">
 jx:each(items="apiData" var="data" lastCell="F30")
 jx:each(items="apiData2" var="data2" lastCell="F30")
-jx:each(items="apiData3" var="data3" lastCell="F30")
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+jx:each(items="apiData3" var="data3" lastCell="F8")
 </t>
         </r>
       </text>
@@ -144,18 +167,18 @@
     <t>${data3.totalMoney}</t>
   </si>
   <si>
-    <t>x</t>
+    <t xml:space="preserve">Tổng tiền hủy </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0\ [$VND]"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -226,8 +249,22 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -264,20 +301,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -294,40 +319,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -337,8 +361,47 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -359,9 +422,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -399,9 +462,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,7 +499,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -471,7 +534,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -644,135 +707,164 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="38.44140625" customWidth="1"/>
-    <col min="3" max="3" width="38.88671875" customWidth="1"/>
-    <col min="4" max="4" width="38.109375" customWidth="1"/>
-    <col min="5" max="5" width="37.21875" customWidth="1"/>
-    <col min="6" max="6" width="47.109375" customWidth="1"/>
+    <col min="2" max="2" width="48.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" style="4" customWidth="1"/>
+    <col min="4" max="4" width="47.44140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="44.88671875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="52.21875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="14"/>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
+      <c r="A1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4"/>
-      <c r="B3" s="1" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="6" t="s">
+    <row r="4" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" spans="1:6" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
+      <c r="A5" s="3"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+    <row r="6" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
     </row>
     <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="B8" s="10" t="s">
+    <row r="8" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="F8" s="22" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="10">
+        <f>SUM(F8)</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C11" s="11"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D12" t="s">
-        <v>22</v>
-      </c>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D20" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Fix bug : export excel thống kê
</commit_message>
<xml_diff>
--- a/BE/src/main/resources/jxls/api_data.xlsx
+++ b/BE/src/main/resources/jxls/api_data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720"/>
   </bookViews>
   <sheets>
     <sheet name="Thống kê" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="F30")</t>
+jx:area(lastCell="G10")</t>
         </r>
       </text>
     </comment>
@@ -63,8 +63,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="apiData" var="data" lastCell="F30")
-jx:each(items="apiData2" var="data2" lastCell="F30")
+jx:each(items="apiData" var="data" lastCell="G10")
+jx:each(items="apiData2" var="data2" lastCell="G10")
 </t>
         </r>
       </text>
@@ -89,7 +89,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="apiData3" var="data3" lastCell="F8")
+jx:each(items="apiData3" var="data3" lastCell="G8")
 </t>
         </r>
       </text>
@@ -99,17 +99,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>Tổng Đơn Hàng Tháng Này</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Tổng Doanh Thu Tháng Này</t>
   </si>
   <si>
-    <t>Tổng Đơn Hàng Hôm Nay</t>
-  </si>
-  <si>
     <t>Tổng Doanh Thu Hôm Nay</t>
   </si>
   <si>
@@ -168,6 +162,18 @@
   </si>
   <si>
     <t xml:space="preserve">Tổng tiền hủy </t>
+  </si>
+  <si>
+    <t>Thời Gian</t>
+  </si>
+  <si>
+    <t>${data3.lastModifiedDate}</t>
+  </si>
+  <si>
+    <t>Tổng Đơn Tháng Này</t>
+  </si>
+  <si>
+    <t>Tổng Đơn  Hôm Nay</t>
   </si>
 </sst>
 </file>
@@ -178,7 +184,7 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="#,##0\ [$VND]"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,13 +223,6 @@
     <font>
       <b/>
       <sz val="16"/>
-      <color theme="4" tint="-0.249977111117893"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="16"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -251,15 +250,29 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="18"/>
+      <color theme="4" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="18"/>
       <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -302,7 +315,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -334,14 +347,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -355,52 +381,67 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -708,169 +749,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.5546875" customWidth="1"/>
-    <col min="2" max="2" width="48.6640625" style="4" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="47.44140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="44.88671875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="52.21875" style="4" customWidth="1"/>
+    <col min="1" max="1" width="2.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="43.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="52.28515625" style="4" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-    </row>
-    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="1" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+    </row>
+    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+    </row>
+    <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="11" t="s">
+      <c r="G4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+    </row>
+    <row r="6" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+    </row>
+    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="29" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="F9" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="23">
+        <f>SUM(G8)</f>
         <v>0</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-    </row>
-    <row r="7" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="40.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" s="10">
-        <f>SUM(F8)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C11" s="1"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.3">
-      <c r="D20" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10" s="1"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="C6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update export thống kê + fix bug trả hàng
</commit_message>
<xml_diff>
--- a/BE/src/main/resources/jxls/api_data.xlsx
+++ b/BE/src/main/resources/jxls/api_data.xlsx
@@ -39,7 +39,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="G10")</t>
+jx:area(lastCell="H10")</t>
         </r>
       </text>
     </comment>
@@ -63,8 +63,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="apiData" var="data" lastCell="G10")
-jx:each(items="apiData2" var="data2" lastCell="G10")
+jx:each(items="apiData" var="data" lastCell="H10")
+jx:each(items="apiData2" var="data2" lastCell="H10")
 </t>
         </r>
       </text>
@@ -89,7 +89,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="apiData3" var="data3" lastCell="G8")
+jx:each(items="apiData3" var="data3" lastCell="H8")
 </t>
         </r>
       </text>
@@ -99,7 +99,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Tổng Doanh Thu Tháng Này</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t>Tổng Đơn  Hôm Nay</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>${data3.note}</t>
   </si>
 </sst>
 </file>
@@ -365,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -380,7 +386,6 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -402,7 +407,6 @@
     <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -428,6 +432,10 @@
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -439,9 +447,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -749,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -764,10 +769,10 @@
     <col min="5" max="5" width="42.42578125" style="4" customWidth="1"/>
     <col min="6" max="6" width="44.85546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="52.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="22.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24"/>
       <c r="B1" s="24"/>
       <c r="C1" s="24"/>
@@ -775,8 +780,9 @@
       <c r="E1" s="24"/>
       <c r="F1" s="24"/>
       <c r="G1" s="24"/>
-    </row>
-    <row r="2" spans="1:7" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H1" s="23"/>
+    </row>
+    <row r="2" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
@@ -787,54 +793,57 @@
       <c r="F2" s="27"/>
       <c r="G2" s="27"/>
     </row>
-    <row r="3" spans="1:7" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
-      <c r="B3" s="20"/>
-      <c r="C3" s="15" t="s">
+      <c r="B3" s="18"/>
+      <c r="C3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="7" t="s">
+      <c r="B4" s="19"/>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="14"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-    </row>
-    <row r="6" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="28" t="s">
         <v>9</v>
       </c>
@@ -843,72 +852,78 @@
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
     </row>
-    <row r="7" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="29" t="s">
+    <row r="7" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="29" t="s">
+      <c r="C7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="29" t="s">
+      <c r="D7" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="29" t="s">
+      <c r="E7" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="29" t="s">
+      <c r="G7" s="22" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="H7" s="22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="F9" s="18" t="s">
+      <c r="H8" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="F9" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="21">
         <f>SUM(G8)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D10" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" s="5"/>
     </row>
     <row r="17" spans="5:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix in hóa đơn send email
</commit_message>
<xml_diff>
--- a/BE/src/main/resources/jxls/api_data.xlsx
+++ b/BE/src/main/resources/jxls/api_data.xlsx
@@ -371,7 +371,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -448,6 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -757,7 +760,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,7 +898,7 @@
       <c r="G8" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="29" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>